<commit_message>
Attendance up to date NOV 3, TA Meeting
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week10.xlsx
+++ b/Admin/Gaby/TimeSheet_Week10.xlsx
@@ -364,11 +364,11 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -464,7 +464,9 @@
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -473,7 +475,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="13" t="n">
         <f aca="false">SUM(B6:H6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="9"/>
     </row>
@@ -483,14 +485,16 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
       <c r="H7" s="11"/>
       <c r="I7" s="13" t="n">
         <f aca="false">SUM(B7:H7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="9"/>
     </row>
@@ -502,12 +506,14 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="G8" s="12"/>
       <c r="H8" s="11"/>
       <c r="I8" s="13" t="n">
         <f aca="false">SUM(B8:H8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -554,11 +560,13 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="H11" s="11"/>
       <c r="I11" s="13" t="n">
         <f aca="false">SUM(B11:H11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -589,10 +597,12 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11" t="n">
+        <v>4</v>
+      </c>
       <c r="I13" s="13" t="n">
         <f aca="false">SUM(B13:H13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="9"/>
     </row>
@@ -602,7 +612,7 @@
       </c>
       <c r="B14" s="13" t="n">
         <f aca="false">SUM(B6:B13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="13" t="n">
         <f aca="false">SUM(C6:C13)</f>
@@ -610,7 +620,7 @@
       </c>
       <c r="D14" s="13" t="n">
         <f aca="false">SUM(D6:D13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="13" t="n">
         <f aca="false">SUM(E6:E13)</f>
@@ -618,19 +628,19 @@
       </c>
       <c r="F14" s="13" t="n">
         <f aca="false">SUM(F6:F13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="13" t="n">
         <f aca="false">SUM(G6:G13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="13" t="n">
         <f aca="false">SUM(H6:H13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I14" s="13" t="n">
         <f aca="false">SUM(I6:I13)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>